<commit_message>
Add ACME_Performer project and update ACME_Dispatcher
Added the full ACME_Performer RPA project including workflows, framework files, configuration. Updated ACME_Dispatcher workflows, configuration, and binaries to support new features and improvements.
</commit_message>
<xml_diff>
--- a/RPA Projects/ACME_Dispatcher/Data/Config.xlsx
+++ b/RPA Projects/ACME_Dispatcher/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khalil\Documents\UiPath\ACME_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C762DA84-A1D9-4370-AEC9-3B2F7264A0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E6A83F-A0F8-4F01-9208-EEB3631571CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -168,9 +168,6 @@
     <t>ITI</t>
   </si>
   <si>
-    <t>Base64_URL</t>
-  </si>
-  <si>
     <t>Name of the credential asset (used by Get Credentials)</t>
   </si>
   <si>
@@ -186,15 +183,6 @@
     <t>https://acme-test.uipath.com/login</t>
   </si>
   <si>
-    <t>https://www.base64encode.org/</t>
-  </si>
-  <si>
-    <t>Acme_URL_WorkItem</t>
-  </si>
-  <si>
-    <t>https://acme-test.uipath.com/work-items/</t>
-  </si>
-  <si>
     <t>ReportFolder</t>
   </si>
   <si>
@@ -223,6 +211,12 @@
   </si>
   <si>
     <t>ACME Dispatcher – {RunId} – {Success}/{Total} queued</t>
+  </si>
+  <si>
+    <t>Acme_URL_WorkItems</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items</t>
   </si>
 </sst>
 </file>
@@ -613,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -666,7 +660,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -691,7 +685,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -710,78 +704,70 @@
         <v>43</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
+        <v>54</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="30">
       <c r="A15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="30">
+        <v>55</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="6" t="b">
+        <v>56</v>
+      </c>
+      <c r="B16" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -790,11 +776,10 @@
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1" xr:uid="{39E672C4-DDF5-430A-A552-E6733D9E687B}"/>
     <hyperlink ref="B8" r:id="rId2" xr:uid="{FC9B6E16-103F-45C0-A7F2-E614918F8E21}"/>
-    <hyperlink ref="B10" r:id="rId3" xr:uid="{D1E806C1-8127-4A50-AEC2-71F07D610C0B}"/>
-    <hyperlink ref="B15" r:id="rId4" display="mailto:a.kh1401@outlook.com" xr:uid="{1735E2FA-5A9E-4260-B2EC-5B829FDF8228}"/>
+    <hyperlink ref="B14" r:id="rId3" display="mailto:a.kh1401@outlook.com" xr:uid="{1735E2FA-5A9E-4260-B2EC-5B829FDF8228}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1043,16 +1028,16 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>